<commit_message>
Updated progress report after working on requirement analysis
</commit_message>
<xml_diff>
--- a/ProgressReports/ConnorDougherty_ProgressReport.xlsx
+++ b/ProgressReports/ConnorDougherty_ProgressReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Group Meeting</t>
+  </si>
+  <si>
+    <t>Requirement Analysis Drafting</t>
   </si>
 </sst>
 </file>
@@ -225,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -239,6 +242,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,9 +617,15 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
+      <c r="A3" s="13">
+        <v>42765</v>
+      </c>
+      <c r="B3" s="7">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>

</xml_diff>

<commit_message>
Updated progress report and added user ER diagram
</commit_message>
<xml_diff>
--- a/ProgressReports/ConnorDougherty_ProgressReport.xlsx
+++ b/ProgressReports/ConnorDougherty_ProgressReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Requirement Analysis Drafting</t>
+  </si>
+  <si>
+    <t>ER Diagram</t>
   </si>
 </sst>
 </file>
@@ -584,7 +587,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -628,14 +631,26 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
+      <c r="A4" s="13">
+        <v>42766</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="13">
+        <v>42767</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>

</xml_diff>

<commit_message>
Updated progress report and created tables for registered user
</commit_message>
<xml_diff>
--- a/ProgressReports/ConnorDougherty_ProgressReport.xlsx
+++ b/ProgressReports/ConnorDougherty_ProgressReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>ER Diagram and Report Editing</t>
+  </si>
+  <si>
+    <t>Schema Refinement and Table Creation</t>
   </si>
 </sst>
 </file>
@@ -590,7 +593,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,14 +670,26 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="13">
+        <v>42791</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="13">
+        <v>42792</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>

</xml_diff>

<commit_message>
Updated rating system schema, updated credit card table, added billing address table, updated progress report
</commit_message>
<xml_diff>
--- a/ProgressReports/ConnorDougherty_ProgressReport.xlsx
+++ b/ProgressReports/ConnorDougherty_ProgressReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>Adding and Updating SQL tables</t>
+  </si>
+  <si>
+    <t>Updating SQL tables and Report</t>
+  </si>
+  <si>
+    <t>Updating Rating System Schema</t>
   </si>
 </sst>
 </file>
@@ -599,7 +605,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,14 +726,26 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="13">
+        <v>42795</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="13">
+        <v>42796</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>

</xml_diff>

<commit_message>
Added quantity to sales_transaction, made buyer_id foreign key, updated progress report
</commit_message>
<xml_diff>
--- a/ProgressReports/ConnorDougherty_ProgressReport.xlsx
+++ b/ProgressReports/ConnorDougherty_ProgressReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Updating and refining SQL tables</t>
+  </si>
+  <si>
+    <t>Tested and Fixed SQL files</t>
   </si>
 </sst>
 </file>
@@ -608,7 +611,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,9 +765,15 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="13">
+        <v>42796</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>

</xml_diff>